<commit_message>
fixing one spanish unilemmma
</commit_message>
<xml_diff>
--- a/raw_data/Spanish_WG/[Spanish_WG].xlsx
+++ b/raw_data/Spanish_WG/[Spanish_WG].xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25160" windowHeight="13780" tabRatio="988"/>
@@ -9713,8 +9713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A326" workbookViewId="0">
-      <selection activeCell="H349" sqref="H349"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="K281" sqref="K281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -21057,7 +21057,7 @@
         <v>1427</v>
       </c>
       <c r="H420" t="s">
-        <v>660</v>
+        <v>3015</v>
       </c>
       <c r="J420" s="5"/>
     </row>
@@ -49969,7 +49969,7 @@
         <v>0</v>
       </c>
       <c r="H706" s="4" t="str">
-        <f t="shared" ref="H706:H769" si="35">IF(I706=I705,"FLAG","")</f>
+        <f t="shared" ref="H706:H768" si="35">IF(I706=I705,"FLAG","")</f>
         <v/>
       </c>
       <c r="I706" s="11" t="s">

</xml_diff>